<commit_message>
updated API calls for chestIds
</commit_message>
<xml_diff>
--- a/data/userIds.xlsx
+++ b/data/userIds.xlsx
@@ -37,7 +37,7 @@
     <t>III</t>
   </si>
   <si>
-    <t>English</t>
+    <t>Science</t>
   </si>
 </sst>
 </file>
@@ -987,7 +987,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="3"/>

</xml_diff>